<commit_message>
Added Test documentation forms Added FileOutputStream to Time_Observer and all concrete classes. Added null check for FileOutputStream and updated JUnit tests, reran
</commit_message>
<xml_diff>
--- a/app/src/test/java/Observers/Check_State_29_Aug_7pm.xlsx
+++ b/app/src/test/java/Observers/Check_State_29_Aug_7pm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Uni 2018\Sem 2\Capstone\Testing\Observers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AFD257-114F-4E49-88CD-37641F12FDD7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33360AD8-2E93-4C37-BDDD-27C8F12A7D8D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{A330BECD-E836-4AC6-938E-7E613B009CCC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{A330BECD-E836-4AC6-938E-7E613B009CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Test Date: 29th August 2018</t>
   </si>
   <si>
-    <t>Purpose: Unit test the locial structure of the Check_State Class and its Interface</t>
-  </si>
-  <si>
     <t>Assumptions/Dependencies: No default value is allowed</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>NullPointerException thrown from the Input_Stream check in the resulting if statement check and cannot check if the Output_Stream exception throw works</t>
+  </si>
+  <si>
+    <t>Purpose: Unit test the logical structure of the Check_State Class and its Interface</t>
   </si>
 </sst>
 </file>
@@ -183,6 +183,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -200,12 +206,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3386EA7-E985-4B0C-876A-4522744B2EB5}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,69 +535,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -617,91 +617,91 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>